<commit_message>
Fixed Regex bug, updated QB starter definition
</commit_message>
<xml_diff>
--- a/DraftSheets/2020_DRAFT_SHEET.xlsx
+++ b/DraftSheets/2020_DRAFT_SHEET.xlsx
@@ -2776,13 +2776,13 @@
         <v>0.4375</v>
       </c>
       <c r="L25" t="n">
-        <v>1.993749999999999</v>
+        <v>2.809374999999996</v>
       </c>
       <c r="M25" t="n">
         <v>0.9333333333333333</v>
       </c>
       <c r="N25" t="n">
-        <v>0.6436595897370865</v>
+        <v>0.6933612743506347</v>
       </c>
       <c r="O25" t="n">
         <v>25.4</v>
@@ -4470,13 +4470,13 @@
         <v>0.5625</v>
       </c>
       <c r="L43" t="n">
-        <v>1.893750000000001</v>
+        <v>2.709374999999998</v>
       </c>
       <c r="M43" t="n">
         <v>0.9375</v>
       </c>
       <c r="N43" t="n">
-        <v>0.6786044041487267</v>
+        <v>0.7211247851537042</v>
       </c>
       <c r="O43" t="n">
         <v>25.3</v>
@@ -5033,16 +5033,16 @@
         </is>
       </c>
       <c r="K49" t="n">
-        <v>0.5625</v>
+        <v>0.625</v>
       </c>
       <c r="L49" t="n">
-        <v>0.9937499999999986</v>
+        <v>1.809374999999996</v>
       </c>
       <c r="M49" t="n">
         <v>0.875</v>
       </c>
       <c r="N49" t="n">
-        <v>0.6299605249474366</v>
+        <v>0.6786044041487267</v>
       </c>
       <c r="O49" t="n">
         <v>24.4</v>
@@ -5414,13 +5414,13 @@
         <v>0.4375</v>
       </c>
       <c r="L53" t="n">
-        <v>-0.6062499999999993</v>
+        <v>0.2093749999999979</v>
       </c>
       <c r="M53" t="n">
         <v>0.8666666666666667</v>
       </c>
       <c r="N53" t="n">
-        <v>0.4054801330382267</v>
+        <v>0.5108729549290354</v>
       </c>
       <c r="O53" t="n">
         <v>22.8</v>
@@ -6174,7 +6174,7 @@
         <v>0.1875</v>
       </c>
       <c r="L61" t="n">
-        <v>4.293749999999999</v>
+        <v>5.109374999999996</v>
       </c>
       <c r="M61" t="n">
         <v>0.8</v>
@@ -6749,10 +6749,10 @@
         </is>
       </c>
       <c r="K67" t="n">
-        <v>0.4375</v>
+        <v>0.5</v>
       </c>
       <c r="L67" t="n">
-        <v>-0.1062499999999993</v>
+        <v>0.7093749999999979</v>
       </c>
       <c r="M67" t="n">
         <v>0.8125</v>
@@ -6939,16 +6939,16 @@
         </is>
       </c>
       <c r="K69" t="n">
-        <v>0.6875</v>
+        <v>0.75</v>
       </c>
       <c r="L69" t="n">
-        <v>0.7937499999999993</v>
+        <v>1.609374999999996</v>
       </c>
       <c r="M69" t="n">
         <v>0.9375</v>
       </c>
       <c r="N69" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O69" t="n">
         <v>24.2</v>
@@ -7229,10 +7229,10 @@
         </is>
       </c>
       <c r="K72" t="n">
-        <v>0.375</v>
+        <v>0.5625</v>
       </c>
       <c r="L72" t="n">
-        <v>-0.5062500000000014</v>
+        <v>0.3093749999999957</v>
       </c>
       <c r="M72" t="n">
         <v>0.9333333333333333</v>
@@ -8453,10 +8453,10 @@
         </is>
       </c>
       <c r="K85" t="n">
-        <v>0.375</v>
+        <v>0.4375</v>
       </c>
       <c r="L85" t="n">
-        <v>-1.506250000000001</v>
+        <v>-0.6906250000000043</v>
       </c>
       <c r="M85" t="n">
         <v>0.8125</v>
@@ -8643,13 +8643,13 @@
         </is>
       </c>
       <c r="K87" t="n">
-        <v>0.4375</v>
+        <v>0.5</v>
       </c>
       <c r="L87" t="n">
-        <v>-1.506250000000001</v>
+        <v>-0.6906250000000043</v>
       </c>
       <c r="M87" t="n">
-        <v>0.625</v>
+        <v>0.6875</v>
       </c>
       <c r="N87" t="n">
         <v>0.6299605249474366</v>
@@ -9324,7 +9324,7 @@
         <v>0.0625</v>
       </c>
       <c r="L94" t="n">
-        <v>-15.90625</v>
+        <v>-15.090625</v>
       </c>
       <c r="M94" t="n">
         <v>0.2666666666666667</v>
@@ -9793,13 +9793,13 @@
         </is>
       </c>
       <c r="K99" t="n">
-        <v>0.125</v>
+        <v>0.3125</v>
       </c>
       <c r="L99" t="n">
-        <v>-6.506250000000001</v>
+        <v>-5.690625000000004</v>
       </c>
       <c r="M99" t="n">
-        <v>0.625</v>
+        <v>0.6875</v>
       </c>
       <c r="N99" t="n">
         <v>0</v>
@@ -10550,7 +10550,7 @@
         <v>0.125</v>
       </c>
       <c r="L107" t="n">
-        <v>-5.506250000000001</v>
+        <v>-4.690625000000004</v>
       </c>
       <c r="M107" t="n">
         <v>0.7</v>
@@ -11779,10 +11779,10 @@
         </is>
       </c>
       <c r="K120" t="n">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="L120" t="n">
-        <v>-5.106249999999999</v>
+        <v>-4.290625000000002</v>
       </c>
       <c r="M120" t="n">
         <v>0.5625</v>
@@ -12063,13 +12063,13 @@
         </is>
       </c>
       <c r="K123" t="n">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="L123" t="n">
-        <v>-3.40625</v>
+        <v>-2.590625000000003</v>
       </c>
       <c r="M123" t="n">
-        <v>0.75</v>
+        <v>0.8125</v>
       </c>
       <c r="N123" t="n">
         <v>0.3968502629920499</v>
@@ -13014,13 +13014,13 @@
         <v>0.1875</v>
       </c>
       <c r="L133" t="n">
-        <v>-7.40625</v>
+        <v>-6.590625000000003</v>
       </c>
       <c r="M133" t="n">
+        <v>0.5625</v>
+      </c>
+      <c r="N133" t="n">
         <v>0.5</v>
-      </c>
-      <c r="N133" t="n">
-        <v>0</v>
       </c>
       <c r="O133" t="n">
         <v>16</v>
@@ -13204,7 +13204,7 @@
         <v>0.0625</v>
       </c>
       <c r="L135" t="n">
-        <v>-9.40625</v>
+        <v>-8.590625000000003</v>
       </c>
       <c r="M135" t="n">
         <v>0.5</v>
@@ -13391,10 +13391,10 @@
         </is>
       </c>
       <c r="K137" t="n">
-        <v>0.1875</v>
+        <v>0.25</v>
       </c>
       <c r="L137" t="n">
-        <v>-7.306249999999999</v>
+        <v>-6.490625000000001</v>
       </c>
       <c r="M137" t="n">
         <v>0.6</v>
@@ -13866,10 +13866,10 @@
         <v>0.1875</v>
       </c>
       <c r="L142" t="n">
-        <v>-4.90625</v>
+        <v>-4.090625000000003</v>
       </c>
       <c r="M142" t="n">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="N142" t="n">
         <v>0</v>
@@ -14728,7 +14728,7 @@
         <v>0</v>
       </c>
       <c r="L151" t="n">
-        <v>-9.80625</v>
+        <v>-8.990625000000003</v>
       </c>
       <c r="M151" t="n">
         <v>0.3571428571428572</v>
@@ -15207,13 +15207,13 @@
         </is>
       </c>
       <c r="K156" t="n">
-        <v>0.1875</v>
+        <v>0.375</v>
       </c>
       <c r="L156" t="n">
-        <v>-5.806249999999999</v>
+        <v>-4.990625000000001</v>
       </c>
       <c r="M156" t="n">
-        <v>0.5625</v>
+        <v>0.625</v>
       </c>
       <c r="N156" t="n">
         <v>0.3968502629920499</v>
@@ -17166,7 +17166,7 @@
         <v>0.0625</v>
       </c>
       <c r="L176" t="n">
-        <v>-11.30625</v>
+        <v>-10.490625</v>
       </c>
       <c r="M176" t="n">
         <v>0.25</v>
@@ -19112,7 +19112,7 @@
         <v>0.1875</v>
       </c>
       <c r="L196" t="n">
-        <v>-5.606249999999999</v>
+        <v>-4.790625000000002</v>
       </c>
       <c r="M196" t="n">
         <v>0.5833333333333334</v>
@@ -19614,10 +19614,10 @@
         <v>0.3125</v>
       </c>
       <c r="L201" t="n">
-        <v>-6.506250000000001</v>
+        <v>-5.690625000000004</v>
       </c>
       <c r="M201" t="n">
-        <v>0.5333333333333333</v>
+        <v>0.6</v>
       </c>
       <c r="N201" t="n">
         <v>0</v>
@@ -21174,7 +21174,7 @@
         <v>0.3125</v>
       </c>
       <c r="L217" t="n">
-        <v>-5.40625</v>
+        <v>-4.590625000000003</v>
       </c>
       <c r="M217" t="n">
         <v>0.6</v>
@@ -22480,7 +22480,7 @@
         <v>0.125</v>
       </c>
       <c r="L230" t="n">
-        <v>-14.00625</v>
+        <v>-13.190625</v>
       </c>
       <c r="M230" t="n">
         <v>0.25</v>
@@ -22868,7 +22868,7 @@
         <v>0</v>
       </c>
       <c r="L234" t="n">
-        <v>-22.60625</v>
+        <v>-21.790625</v>
       </c>
       <c r="M234" t="n">
         <v>0</v>
@@ -26185,10 +26185,10 @@
         </is>
       </c>
       <c r="K268" t="n">
-        <v>0.5</v>
+        <v>0.5625</v>
       </c>
       <c r="L268" t="n">
-        <v>0.09375</v>
+        <v>0.9093749999999972</v>
       </c>
       <c r="M268" t="n">
         <v>0.9375</v>
@@ -28252,7 +28252,7 @@
         <v>0.0625</v>
       </c>
       <c r="L289" t="n">
-        <v>-11.80625</v>
+        <v>-10.990625</v>
       </c>
       <c r="M289" t="n">
         <v>0.3333333333333333</v>
@@ -28546,13 +28546,13 @@
         <v>0.1875</v>
       </c>
       <c r="L292" t="n">
-        <v>-8.30625</v>
+        <v>-7.490625000000003</v>
       </c>
       <c r="M292" t="n">
         <v>0.3846153846153846</v>
       </c>
       <c r="N292" t="n">
-        <v>0</v>
+        <v>0.4252903702829902</v>
       </c>
       <c r="O292" t="n">
         <v>15.1</v>
@@ -28642,7 +28642,7 @@
         <v>0.125</v>
       </c>
       <c r="L293" t="n">
-        <v>-6.606249999999999</v>
+        <v>-5.790625000000002</v>
       </c>
       <c r="M293" t="n">
         <v>0.5333333333333333</v>
@@ -29295,7 +29295,7 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>100</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
@@ -29389,7 +29389,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>101</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
@@ -29483,7 +29483,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>102</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
@@ -29577,7 +29577,7 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>103</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
@@ -29671,7 +29671,7 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>104</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
@@ -30057,7 +30057,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>105</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
@@ -30349,7 +30349,7 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>106</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
@@ -30443,7 +30443,7 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>107</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
@@ -30580,7 +30580,7 @@
         <v>0</v>
       </c>
       <c r="L313" t="n">
-        <v>-18.90625</v>
+        <v>-18.090625</v>
       </c>
       <c r="M313" t="n">
         <v>0</v>
@@ -30639,7 +30639,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>108</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
@@ -30931,7 +30931,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>109</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
@@ -32401,7 +32401,7 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>110</t>
         </is>
       </c>
       <c r="E332" t="inlineStr">
@@ -32699,7 +32699,7 @@
       </c>
       <c r="D335" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>111</t>
         </is>
       </c>
       <c r="E335" t="inlineStr">
@@ -32887,7 +32887,7 @@
       </c>
       <c r="D337" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>112</t>
         </is>
       </c>
       <c r="E337" t="inlineStr">
@@ -33169,7 +33169,7 @@
       </c>
       <c r="D340" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>113</t>
         </is>
       </c>
       <c r="E340" t="inlineStr">
@@ -33457,7 +33457,7 @@
       </c>
       <c r="D343" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>114</t>
         </is>
       </c>
       <c r="E343" t="inlineStr">
@@ -33786,10 +33786,10 @@
         <v>0.0625</v>
       </c>
       <c r="L346" t="n">
-        <v>-10.30625</v>
+        <v>-9.490625000000003</v>
       </c>
       <c r="M346" t="n">
-        <v>0.3636363636363636</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="N346" t="n">
         <v>0</v>
@@ -33845,7 +33845,7 @@
       </c>
       <c r="D347" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>115</t>
         </is>
       </c>
       <c r="E347" t="inlineStr">
@@ -34515,7 +34515,7 @@
       </c>
       <c r="D354" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>116</t>
         </is>
       </c>
       <c r="E354" t="inlineStr">
@@ -34713,7 +34713,7 @@
       </c>
       <c r="D356" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>117</t>
         </is>
       </c>
       <c r="E356" t="inlineStr">
@@ -34901,7 +34901,7 @@
       </c>
       <c r="D358" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>100</t>
         </is>
       </c>
       <c r="E358" t="inlineStr">
@@ -35193,7 +35193,7 @@
       </c>
       <c r="D361" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>101</t>
         </is>
       </c>
       <c r="E361" t="inlineStr">
@@ -35293,7 +35293,7 @@
       </c>
       <c r="D362" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>118</t>
         </is>
       </c>
       <c r="E362" t="inlineStr">
@@ -35387,7 +35387,7 @@
       </c>
       <c r="D363" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>102</t>
         </is>
       </c>
       <c r="E363" t="inlineStr">
@@ -35481,7 +35481,7 @@
       </c>
       <c r="D364" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>103</t>
         </is>
       </c>
       <c r="E364" t="inlineStr">
@@ -35779,7 +35779,7 @@
       </c>
       <c r="D367" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>104</t>
         </is>
       </c>
       <c r="E367" t="inlineStr">
@@ -35977,7 +35977,7 @@
       </c>
       <c r="D369" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>105</t>
         </is>
       </c>
       <c r="E369" t="inlineStr">
@@ -36077,7 +36077,7 @@
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>119</t>
         </is>
       </c>
       <c r="E370" t="inlineStr">
@@ -36265,7 +36265,7 @@
       </c>
       <c r="D372" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>120</t>
         </is>
       </c>
       <c r="E372" t="inlineStr">
@@ -36359,7 +36359,7 @@
       </c>
       <c r="D373" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>121</t>
         </is>
       </c>
       <c r="E373" t="inlineStr">
@@ -36453,7 +36453,7 @@
       </c>
       <c r="D374" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>122</t>
         </is>
       </c>
       <c r="E374" t="inlineStr">
@@ -37057,7 +37057,7 @@
       </c>
       <c r="D380" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>106</t>
         </is>
       </c>
       <c r="E380" t="inlineStr">
@@ -37253,7 +37253,7 @@
       </c>
       <c r="D382" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>123</t>
         </is>
       </c>
       <c r="E382" t="inlineStr">
@@ -37347,7 +37347,7 @@
       </c>
       <c r="D383" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>124</t>
         </is>
       </c>
       <c r="E383" t="inlineStr">
@@ -37541,7 +37541,7 @@
       </c>
       <c r="D385" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>125</t>
         </is>
       </c>
       <c r="E385" t="inlineStr">
@@ -37635,7 +37635,7 @@
       </c>
       <c r="D386" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>126</t>
         </is>
       </c>
       <c r="E386" t="inlineStr">
@@ -37735,7 +37735,7 @@
       </c>
       <c r="D387" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>127</t>
         </is>
       </c>
       <c r="E387" t="inlineStr">
@@ -37931,7 +37931,7 @@
       </c>
       <c r="D389" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>128</t>
         </is>
       </c>
       <c r="E389" t="inlineStr">
@@ -38025,7 +38025,7 @@
       </c>
       <c r="D390" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>129</t>
         </is>
       </c>
       <c r="E390" t="inlineStr">
@@ -38119,7 +38119,7 @@
       </c>
       <c r="D391" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>107</t>
         </is>
       </c>
       <c r="E391" t="inlineStr">
@@ -38213,7 +38213,7 @@
       </c>
       <c r="D392" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>130</t>
         </is>
       </c>
       <c r="E392" t="inlineStr">
@@ -38313,7 +38313,7 @@
       </c>
       <c r="D393" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>131</t>
         </is>
       </c>
       <c r="E393" t="inlineStr">
@@ -38407,7 +38407,7 @@
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>108</t>
         </is>
       </c>
       <c r="E394" t="inlineStr">
@@ -38803,7 +38803,7 @@
       </c>
       <c r="D398" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>132</t>
         </is>
       </c>
       <c r="E398" t="inlineStr">
@@ -38897,7 +38897,7 @@
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>133</t>
         </is>
       </c>
       <c r="E399" t="inlineStr">
@@ -38991,7 +38991,7 @@
       </c>
       <c r="D400" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>134</t>
         </is>
       </c>
       <c r="E400" t="inlineStr">
@@ -39179,7 +39179,7 @@
       </c>
       <c r="D402" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>109</t>
         </is>
       </c>
       <c r="E402" t="inlineStr">
@@ -39273,7 +39273,7 @@
       </c>
       <c r="D403" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>110</t>
         </is>
       </c>
       <c r="E403" t="inlineStr">
@@ -39579,7 +39579,7 @@
       </c>
       <c r="D406" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>135</t>
         </is>
       </c>
       <c r="E406" t="inlineStr">
@@ -39673,7 +39673,7 @@
       </c>
       <c r="D407" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>111</t>
         </is>
       </c>
       <c r="E407" t="inlineStr">
@@ -39977,7 +39977,7 @@
       </c>
       <c r="D410" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>136</t>
         </is>
       </c>
       <c r="E410" t="inlineStr">
@@ -40077,7 +40077,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>137</t>
         </is>
       </c>
       <c r="E411" t="inlineStr">
@@ -40555,7 +40555,7 @@
       </c>
       <c r="D416" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>112</t>
         </is>
       </c>
       <c r="E416" t="inlineStr">
@@ -40649,7 +40649,7 @@
       </c>
       <c r="D417" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>113</t>
         </is>
       </c>
       <c r="E417" t="inlineStr">
@@ -40743,7 +40743,7 @@
       </c>
       <c r="D418" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>114</t>
         </is>
       </c>
       <c r="E418" t="inlineStr">
@@ -40837,7 +40837,7 @@
       </c>
       <c r="D419" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>138</t>
         </is>
       </c>
       <c r="E419" t="inlineStr">
@@ -40931,7 +40931,7 @@
       </c>
       <c r="D420" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>139</t>
         </is>
       </c>
       <c r="E420" t="inlineStr">
@@ -41031,7 +41031,7 @@
       </c>
       <c r="D421" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>140</t>
         </is>
       </c>
       <c r="E421" t="inlineStr">
@@ -41125,7 +41125,7 @@
       </c>
       <c r="D422" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>115</t>
         </is>
       </c>
       <c r="E422" t="inlineStr">
@@ -41225,7 +41225,7 @@
       </c>
       <c r="D423" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>141</t>
         </is>
       </c>
       <c r="E423" t="inlineStr">
@@ -41319,7 +41319,7 @@
       </c>
       <c r="D424" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>116</t>
         </is>
       </c>
       <c r="E424" t="inlineStr">
@@ -41450,7 +41450,7 @@
         <v>0.0625</v>
       </c>
       <c r="L425" t="n">
-        <v>-5.106249999999999</v>
+        <v>-4.290625000000002</v>
       </c>
       <c r="M425" t="n">
         <v>0.7777777777777778</v>
@@ -41509,7 +41509,7 @@
       </c>
       <c r="D426" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>117</t>
         </is>
       </c>
       <c r="E426" t="inlineStr">
@@ -41609,7 +41609,7 @@
       </c>
       <c r="D427" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>118</t>
         </is>
       </c>
       <c r="E427" t="inlineStr">
@@ -41703,7 +41703,7 @@
       </c>
       <c r="D428" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>142</t>
         </is>
       </c>
       <c r="E428" t="inlineStr">
@@ -41803,7 +41803,7 @@
       </c>
       <c r="D429" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>143</t>
         </is>
       </c>
       <c r="E429" t="inlineStr">
@@ -41903,7 +41903,7 @@
       </c>
       <c r="D430" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>144</t>
         </is>
       </c>
       <c r="E430" t="inlineStr">
@@ -42091,7 +42091,7 @@
       </c>
       <c r="D432" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>145</t>
         </is>
       </c>
       <c r="E432" t="inlineStr">
@@ -42279,7 +42279,7 @@
       </c>
       <c r="D434" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>119</t>
         </is>
       </c>
       <c r="E434" t="inlineStr">
@@ -42410,7 +42410,7 @@
         <v>0</v>
       </c>
       <c r="L435" t="n">
-        <v>-11.70625</v>
+        <v>-10.890625</v>
       </c>
       <c r="M435" t="n">
         <v>0</v>
@@ -42469,7 +42469,7 @@
       </c>
       <c r="D436" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>120</t>
         </is>
       </c>
       <c r="E436" t="inlineStr">
@@ -42600,10 +42600,10 @@
         <v>0.1875</v>
       </c>
       <c r="L437" t="n">
-        <v>-7.206250000000001</v>
+        <v>-6.390625000000004</v>
       </c>
       <c r="M437" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="N437" t="n">
         <v>0</v>
@@ -42759,7 +42759,7 @@
       </c>
       <c r="D439" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>146</t>
         </is>
       </c>
       <c r="E439" t="inlineStr">
@@ -42953,7 +42953,7 @@
       </c>
       <c r="D441" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>121</t>
         </is>
       </c>
       <c r="E441" t="inlineStr">
@@ -43053,7 +43053,7 @@
       </c>
       <c r="D442" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>147</t>
         </is>
       </c>
       <c r="E442" t="inlineStr">
@@ -43247,7 +43247,7 @@
       </c>
       <c r="D444" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>148</t>
         </is>
       </c>
       <c r="E444" t="inlineStr">
@@ -43341,7 +43341,7 @@
       </c>
       <c r="D445" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>122</t>
         </is>
       </c>
       <c r="E445" t="inlineStr">
@@ -43435,7 +43435,7 @@
       </c>
       <c r="D446" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>123</t>
         </is>
       </c>
       <c r="E446" t="inlineStr">
@@ -43760,7 +43760,7 @@
         <v>0.0625</v>
       </c>
       <c r="L449" t="n">
-        <v>3.393750000000001</v>
+        <v>4.209374999999998</v>
       </c>
       <c r="M449" t="n">
         <v>1</v>
@@ -44013,7 +44013,7 @@
       </c>
       <c r="D452" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>149</t>
         </is>
       </c>
       <c r="E452" t="inlineStr">
@@ -44213,7 +44213,7 @@
       </c>
       <c r="D454" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>150</t>
         </is>
       </c>
       <c r="E454" t="inlineStr">
@@ -44307,7 +44307,7 @@
       </c>
       <c r="D455" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>151</t>
         </is>
       </c>
       <c r="E455" t="inlineStr">
@@ -44495,7 +44495,7 @@
       </c>
       <c r="D457" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>124</t>
         </is>
       </c>
       <c r="E457" t="inlineStr">
@@ -44589,7 +44589,7 @@
       </c>
       <c r="D458" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>152</t>
         </is>
       </c>
       <c r="E458" t="inlineStr">
@@ -44877,7 +44877,7 @@
       </c>
       <c r="D461" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>153</t>
         </is>
       </c>
       <c r="E461" t="inlineStr">
@@ -44971,7 +44971,7 @@
       </c>
       <c r="D462" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>125</t>
         </is>
       </c>
       <c r="E462" t="inlineStr">
@@ -45065,7 +45065,7 @@
       </c>
       <c r="D463" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>126</t>
         </is>
       </c>
       <c r="E463" t="inlineStr">
@@ -45159,7 +45159,7 @@
       </c>
       <c r="D464" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>154</t>
         </is>
       </c>
       <c r="E464" t="inlineStr">
@@ -45253,7 +45253,7 @@
       </c>
       <c r="D465" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>127</t>
         </is>
       </c>
       <c r="E465" t="inlineStr">
@@ -45441,7 +45441,7 @@
       </c>
       <c r="D467" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>155</t>
         </is>
       </c>
       <c r="E467" t="inlineStr">
@@ -45541,7 +45541,7 @@
       </c>
       <c r="D468" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>156</t>
         </is>
       </c>
       <c r="E468" t="inlineStr">
@@ -45735,7 +45735,7 @@
       </c>
       <c r="D470" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>128</t>
         </is>
       </c>
       <c r="E470" t="inlineStr">
@@ -45829,7 +45829,7 @@
       </c>
       <c r="D471" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>157</t>
         </is>
       </c>
       <c r="E471" t="inlineStr">
@@ -45923,7 +45923,7 @@
       </c>
       <c r="D472" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>129</t>
         </is>
       </c>
       <c r="E472" t="inlineStr">
@@ -46017,7 +46017,7 @@
       </c>
       <c r="D473" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>130</t>
         </is>
       </c>
       <c r="E473" t="inlineStr">
@@ -46111,7 +46111,7 @@
       </c>
       <c r="D474" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>158</t>
         </is>
       </c>
       <c r="E474" t="inlineStr">
@@ -46205,7 +46205,7 @@
       </c>
       <c r="D475" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>131</t>
         </is>
       </c>
       <c r="E475" t="inlineStr">
@@ -46299,7 +46299,7 @@
       </c>
       <c r="D476" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>159</t>
         </is>
       </c>
       <c r="E476" t="inlineStr">
@@ -46393,7 +46393,7 @@
       </c>
       <c r="D477" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>132</t>
         </is>
       </c>
       <c r="E477" t="inlineStr">
@@ -46487,7 +46487,7 @@
       </c>
       <c r="D478" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>133</t>
         </is>
       </c>
       <c r="E478" t="inlineStr">
@@ -46581,7 +46581,7 @@
       </c>
       <c r="D479" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>134</t>
         </is>
       </c>
       <c r="E479" t="inlineStr">
@@ -46675,7 +46675,7 @@
       </c>
       <c r="D480" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>160</t>
         </is>
       </c>
       <c r="E480" t="inlineStr">
@@ -46863,7 +46863,7 @@
       </c>
       <c r="D482" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>161</t>
         </is>
       </c>
       <c r="E482" t="inlineStr">
@@ -46963,7 +46963,7 @@
       </c>
       <c r="D483" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>162</t>
         </is>
       </c>
       <c r="E483" t="inlineStr">
@@ -47355,7 +47355,7 @@
       </c>
       <c r="D487" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>163</t>
         </is>
       </c>
       <c r="E487" t="inlineStr">
@@ -47551,7 +47551,7 @@
       </c>
       <c r="D489" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>164</t>
         </is>
       </c>
       <c r="E489" t="inlineStr">
@@ -47651,7 +47651,7 @@
       </c>
       <c r="D490" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>165</t>
         </is>
       </c>
       <c r="E490" t="inlineStr">
@@ -48051,7 +48051,7 @@
       </c>
       <c r="D494" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>166</t>
         </is>
       </c>
       <c r="E494" t="inlineStr">
@@ -48239,7 +48239,7 @@
       </c>
       <c r="D496" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>167</t>
         </is>
       </c>
       <c r="E496" t="inlineStr">
@@ -48333,7 +48333,7 @@
       </c>
       <c r="D497" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>168</t>
         </is>
       </c>
       <c r="E497" t="inlineStr">
@@ -48427,7 +48427,7 @@
       </c>
       <c r="D498" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>169</t>
         </is>
       </c>
       <c r="E498" t="inlineStr">
@@ -48521,7 +48521,7 @@
       </c>
       <c r="D499" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>135</t>
         </is>
       </c>
       <c r="E499" t="inlineStr">
@@ -48717,7 +48717,7 @@
       </c>
       <c r="D501" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>170</t>
         </is>
       </c>
       <c r="E501" t="inlineStr">
@@ -48817,7 +48817,7 @@
       </c>
       <c r="D502" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>171</t>
         </is>
       </c>
       <c r="E502" t="inlineStr">
@@ -49011,7 +49011,7 @@
       </c>
       <c r="D504" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>136</t>
         </is>
       </c>
       <c r="E504" t="inlineStr">
@@ -49111,7 +49111,7 @@
       </c>
       <c r="D505" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>172</t>
         </is>
       </c>
       <c r="E505" t="inlineStr">
@@ -49205,7 +49205,7 @@
       </c>
       <c r="D506" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>173</t>
         </is>
       </c>
       <c r="E506" t="inlineStr">
@@ -49305,7 +49305,7 @@
       </c>
       <c r="D507" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>137</t>
         </is>
       </c>
       <c r="E507" t="inlineStr">
@@ -49399,7 +49399,7 @@
       </c>
       <c r="D508" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>138</t>
         </is>
       </c>
       <c r="E508" t="inlineStr">
@@ -49595,7 +49595,7 @@
       </c>
       <c r="D510" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>139</t>
         </is>
       </c>
       <c r="E510" t="inlineStr">
@@ -49695,7 +49695,7 @@
       </c>
       <c r="D511" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>174</t>
         </is>
       </c>
       <c r="E511" t="inlineStr">
@@ -49789,7 +49789,7 @@
       </c>
       <c r="D512" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>175</t>
         </is>
       </c>
       <c r="E512" t="inlineStr">
@@ -49983,7 +49983,7 @@
       </c>
       <c r="D514" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>176</t>
         </is>
       </c>
       <c r="E514" t="inlineStr">
@@ -50265,7 +50265,7 @@
       </c>
       <c r="D517" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>140</t>
         </is>
       </c>
       <c r="E517" t="inlineStr">
@@ -50365,7 +50365,7 @@
       </c>
       <c r="D518" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>141</t>
         </is>
       </c>
       <c r="E518" t="inlineStr">
@@ -50465,7 +50465,7 @@
       </c>
       <c r="D519" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>177</t>
         </is>
       </c>
       <c r="E519" t="inlineStr">
@@ -50559,7 +50559,7 @@
       </c>
       <c r="D520" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>142</t>
         </is>
       </c>
       <c r="E520" t="inlineStr">
@@ -50653,7 +50653,7 @@
       </c>
       <c r="D521" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>178</t>
         </is>
       </c>
       <c r="E521" t="inlineStr">
@@ -50747,7 +50747,7 @@
       </c>
       <c r="D522" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>143</t>
         </is>
       </c>
       <c r="E522" t="inlineStr">
@@ -50847,7 +50847,7 @@
       </c>
       <c r="D523" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>179</t>
         </is>
       </c>
       <c r="E523" t="inlineStr">
@@ -50941,7 +50941,7 @@
       </c>
       <c r="D524" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>180</t>
         </is>
       </c>
       <c r="E524" t="inlineStr">
@@ -51235,7 +51235,7 @@
       </c>
       <c r="D527" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>181</t>
         </is>
       </c>
       <c r="E527" t="inlineStr">
@@ -51329,7 +51329,7 @@
       </c>
       <c r="D528" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>182</t>
         </is>
       </c>
       <c r="E528" t="inlineStr">
@@ -51423,7 +51423,7 @@
       </c>
       <c r="D529" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>183</t>
         </is>
       </c>
       <c r="E529" t="inlineStr">
@@ -51523,7 +51523,7 @@
       </c>
       <c r="D530" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>184</t>
         </is>
       </c>
       <c r="E530" t="inlineStr">
@@ -51623,7 +51623,7 @@
       </c>
       <c r="D531" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>185</t>
         </is>
       </c>
       <c r="E531" t="inlineStr">
@@ -51717,7 +51717,7 @@
       </c>
       <c r="D532" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>186</t>
         </is>
       </c>
       <c r="E532" t="inlineStr">
@@ -51811,7 +51811,7 @@
       </c>
       <c r="D533" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>144</t>
         </is>
       </c>
       <c r="E533" t="inlineStr">
@@ -51905,7 +51905,7 @@
       </c>
       <c r="D534" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>187</t>
         </is>
       </c>
       <c r="E534" t="inlineStr">
@@ -52005,7 +52005,7 @@
       </c>
       <c r="D535" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>188</t>
         </is>
       </c>
       <c r="E535" t="inlineStr">
@@ -52205,7 +52205,7 @@
       </c>
       <c r="D537" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>189</t>
         </is>
       </c>
       <c r="E537" t="inlineStr">
@@ -52305,7 +52305,7 @@
       </c>
       <c r="D538" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>190</t>
         </is>
       </c>
       <c r="E538" t="inlineStr">
@@ -52505,7 +52505,7 @@
       </c>
       <c r="D540" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>191</t>
         </is>
       </c>
       <c r="E540" t="inlineStr">
@@ -52699,7 +52699,7 @@
       </c>
       <c r="D542" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>192</t>
         </is>
       </c>
       <c r="E542" t="inlineStr">
@@ -52801,7 +52801,7 @@
       </c>
       <c r="D543" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>193</t>
         </is>
       </c>
       <c r="E543" t="inlineStr">

</xml_diff>